<commit_message>
4 - increment Daily scrum meeting
</commit_message>
<xml_diff>
--- a/Increment4/4th increment Daily Scrum Meeting.xlsx
+++ b/Increment4/4th increment Daily Scrum Meeting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\3rd increment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB419B16-7D81-4443-B8F8-9256D69AD26C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CB834ED-DD3C-4FAC-9513-BB8C0B82D293}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12070" windowHeight="4170" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Person</t>
   </si>
@@ -57,9 +57,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>3rd increment______ 30,march,2021 -- 1st,april,2021</t>
-  </si>
-  <si>
     <t>1st Day</t>
   </si>
   <si>
@@ -75,18 +72,9 @@
     <t>nothing</t>
   </si>
   <si>
-    <t>user window design + java part as weel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assigment </t>
-  </si>
-  <si>
     <t xml:space="preserve">fxml file of waiters </t>
   </si>
   <si>
-    <t xml:space="preserve">java </t>
-  </si>
-  <si>
     <t xml:space="preserve">no </t>
   </si>
   <si>
@@ -99,48 +87,12 @@
     <t>issue with database part</t>
   </si>
   <si>
-    <t>struggling to work on her part</t>
-  </si>
-  <si>
-    <t>interface of attendace window</t>
-  </si>
-  <si>
     <t>assigments in other classes</t>
   </si>
   <si>
     <t>table view connect it database</t>
   </si>
   <si>
-    <t>fxml part and creat the functionality for it</t>
-  </si>
-  <si>
-    <t>broke laptop</t>
-  </si>
-  <si>
-    <t>work on functionality of her part</t>
-  </si>
-  <si>
-    <t>worked on functionaly</t>
-  </si>
-  <si>
-    <t>connection with database</t>
-  </si>
-  <si>
-    <t>problems with classes and typing errors</t>
-  </si>
-  <si>
-    <t>woked on interface and functionality of table view</t>
-  </si>
-  <si>
-    <t xml:space="preserve">will work on left functionality </t>
-  </si>
-  <si>
-    <t xml:space="preserve">design of the main page for waiter and add some buttons in the page. design Waiter attendce window. </t>
-  </si>
-  <si>
-    <t>java and database of the waiter main page</t>
-  </si>
-  <si>
     <t>done with the his assigned task</t>
   </si>
   <si>
@@ -150,7 +102,55 @@
     <t>will start working on the 5th increment</t>
   </si>
   <si>
-    <t xml:space="preserve">connect the database with waiter attendce </t>
+    <t>didn’t attend the meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will work on user window design + java part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">will work on java part  </t>
+  </si>
+  <si>
+    <t>still struggling to work on her part</t>
+  </si>
+  <si>
+    <t>will work interface of attendace window</t>
+  </si>
+  <si>
+    <t>will work on functionality of her part</t>
+  </si>
+  <si>
+    <t>her laptop is broke</t>
+  </si>
+  <si>
+    <t>will work on fxml part and creat the functionality for it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woeked on the design of the main page for waiter and add some buttons in the page. design Waiter attendce window. </t>
+  </si>
+  <si>
+    <t>will work on the java and database parts of the waiter's main page</t>
+  </si>
+  <si>
+    <t>will work on the connection of the assigend user stories with database</t>
+  </si>
+  <si>
+    <t>worked on functionality of the assigned user stories</t>
+  </si>
+  <si>
+    <t>faced some issues with classes and some typing errors</t>
+  </si>
+  <si>
+    <t>worked on the interface and functionality of table view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will work on the half of functionality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">connected the database with the waiter's attendance </t>
+  </si>
+  <si>
+    <t>4th increment______ 5th April,2021 -- 8th April,2021</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,6 +354,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,10 +376,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -734,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -745,86 +749,86 @@
     <col min="3" max="3" width="39.4140625" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
     <col min="5" max="5" width="60.83203125" customWidth="1"/>
-    <col min="6" max="6" width="43.58203125" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
@@ -834,103 +838,106 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>9</v>
@@ -943,31 +950,44 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>

</xml_diff>